<commit_message>
ImageUrl included in weapons
</commit_message>
<xml_diff>
--- a/WeaponSystem/WeaponSystem.TestConsoleClient/UnZippedFiles/w.xlsx
+++ b/WeaponSystem/WeaponSystem.TestConsoleClient/UnZippedFiles/w.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pistols" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -43,132 +43,135 @@
     <t>Česká zbrojovka</t>
   </si>
   <si>
+    <t>http://vignette3.wikia.nocookie.net/cswikia/images/6/6a/CZ75go.png/revision/latest/scale-to-width-down/250?cb=20140710231132</t>
+  </si>
+  <si>
+    <t>Desert Eagle</t>
+  </si>
+  <si>
+    <t>Magnum Research</t>
+  </si>
+  <si>
+    <t>http://vignette1.wikia.nocookie.net/cswikia/images/c/cb/Weapon_deagle.png/revision/latest/scale-to-width-down/250?cb=20130903115839</t>
+  </si>
+  <si>
+    <t>Baretta 92 </t>
+  </si>
+  <si>
+    <t>Baretta</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/f/f0/Elitego.png/revision/latest/scale-to-width-down/250?cb=20130813194010</t>
+  </si>
+  <si>
+    <t>Glock-18</t>
+  </si>
+  <si>
+    <t>Glock</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/2/2d/Glockgo.png/revision/latest/scale-to-width-down/250?cb=20130813194200</t>
+  </si>
+  <si>
+    <t>P228</t>
+  </si>
+  <si>
+    <t>SigSauer</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/7/77/P228hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100508112732</t>
+  </si>
+  <si>
+    <t>P250</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/d/d8/P250go.png/revision/latest/scale-to-width-down/250?cb=20130813194341</t>
+  </si>
+  <si>
+    <t>P2000</t>
+  </si>
+  <si>
+    <t>Heckler&amp;Koch</t>
+  </si>
+  <si>
+    <t>http://vignette3.wikia.nocookie.net/cswikia/images/4/4d/P2000go.png/revision/latest/scale-to-width-down/250?cb=20130813194247</t>
+  </si>
+  <si>
+    <t>USP</t>
+  </si>
+  <si>
+    <t>http://vignette1.wikia.nocookie.net/cswikia/images/f/f1/Usphud_cz.png/revision/latest/scale-to-width-down/250?cb=20100505133143</t>
+  </si>
+  <si>
+    <t>.500 S&amp;W</t>
+  </si>
+  <si>
+    <t>Smith&amp;Wesson</t>
+  </si>
+  <si>
+    <t>http://vignette1.wikia.nocookie.net/cswikia/images/3/3c/Csgousp.png/revision/latest/scale-to-width-down/250?cb=20130813110903</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Colt</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/4a/Colt-Python.jpg</t>
+  </si>
+  <si>
+    <t>Automatic-5</t>
+  </si>
+  <si>
+    <t>Browning</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/d/d5/M3hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100728095701</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Benelli</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/0/0b/Nova.png/revision/latest/scale-to-width-down/250?cb=20130813200616</t>
+  </si>
+  <si>
+    <t>M4 Super 90</t>
+  </si>
+  <si>
+    <t>http://vignette1.wikia.nocookie.net/cswikia/images/a/a0/M1014.png/revision/latest/scale-to-width-down/250?cb=20130813200959</t>
+  </si>
+  <si>
+    <t>Saiga-12</t>
+  </si>
+  <si>
+    <t>Izhmash </t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/0/02/Saiga_12_shotgun.jpg</t>
+  </si>
+  <si>
+    <t>MAC-10</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>http://vignette2.wikia.nocookie.net/cswikia/images/5/57/Mac10go.png/revision/latest/scale-to-width-down/250?cb=20130813201114</t>
+  </si>
+  <si>
+    <t>MP5</t>
+  </si>
+  <si>
+    <t>Heckler&amp;Kock</t>
+  </si>
+  <si>
     <t>9mm</t>
   </si>
   <si>
-    <t>http://vignette3.wikia.nocookie.net/cswikia/images/6/6a/CZ75go.png/revision/latest/scale-to-width-down/250?cb=20140710231132</t>
-  </si>
-  <si>
-    <t>Desert Eagle</t>
-  </si>
-  <si>
-    <t>Magnum Research</t>
-  </si>
-  <si>
-    <t>http://vignette1.wikia.nocookie.net/cswikia/images/c/cb/Weapon_deagle.png/revision/latest/scale-to-width-down/250?cb=20130903115839</t>
-  </si>
-  <si>
-    <t>Baretta 92 </t>
-  </si>
-  <si>
-    <t>Baretta</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/f/f0/Elitego.png/revision/latest/scale-to-width-down/250?cb=20130813194010</t>
-  </si>
-  <si>
-    <t>Glock-18</t>
-  </si>
-  <si>
-    <t>Glock</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/2/2d/Glockgo.png/revision/latest/scale-to-width-down/250?cb=20130813194200</t>
-  </si>
-  <si>
-    <t>P228</t>
-  </si>
-  <si>
-    <t>SigSauer</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/7/77/P228hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100508112732</t>
-  </si>
-  <si>
-    <t>P250</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/d/d8/P250go.png/revision/latest/scale-to-width-down/250?cb=20130813194341</t>
-  </si>
-  <si>
-    <t>P2000</t>
-  </si>
-  <si>
-    <t>Heckler&amp;Koch</t>
-  </si>
-  <si>
-    <t>http://vignette3.wikia.nocookie.net/cswikia/images/4/4d/P2000go.png/revision/latest/scale-to-width-down/250?cb=20130813194247</t>
-  </si>
-  <si>
-    <t>USP</t>
-  </si>
-  <si>
-    <t>http://vignette1.wikia.nocookie.net/cswikia/images/f/f1/Usphud_cz.png/revision/latest/scale-to-width-down/250?cb=20100505133143</t>
-  </si>
-  <si>
-    <t>.500 S&amp;W</t>
-  </si>
-  <si>
-    <t>Smith&amp;Wesson</t>
-  </si>
-  <si>
-    <t>http://vignette1.wikia.nocookie.net/cswikia/images/3/3c/Csgousp.png/revision/latest/scale-to-width-down/250?cb=20130813110903</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Colt</t>
-  </si>
-  <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/4/4a/Colt-Python.jpg</t>
-  </si>
-  <si>
-    <t>Automatic-5</t>
-  </si>
-  <si>
-    <t>Browning</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/d/d5/M3hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100728095701</t>
-  </si>
-  <si>
-    <t>Nova</t>
-  </si>
-  <si>
-    <t>Benelli</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/0/0b/Nova.png/revision/latest/scale-to-width-down/250?cb=20130813200616</t>
-  </si>
-  <si>
-    <t>M4 Super 90</t>
-  </si>
-  <si>
-    <t>http://vignette1.wikia.nocookie.net/cswikia/images/a/a0/M1014.png/revision/latest/scale-to-width-down/250?cb=20130813200959</t>
-  </si>
-  <si>
-    <t>Saiga-12</t>
-  </si>
-  <si>
-    <t>Izhmash </t>
-  </si>
-  <si>
-    <t>MAC-10</t>
-  </si>
-  <si>
-    <t>MAC</t>
-  </si>
-  <si>
-    <t>http://vignette2.wikia.nocookie.net/cswikia/images/5/57/Mac10go.png/revision/latest/scale-to-width-down/250?cb=20130813201114</t>
-  </si>
-  <si>
-    <t>MP5</t>
-  </si>
-  <si>
-    <t>Heckler&amp;Kock</t>
-  </si>
-  <si>
     <t>http://vignette3.wikia.nocookie.net/cswikia/images/8/81/Mp5hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100730110854</t>
   </si>
   <si>
@@ -323,6 +326,9 @@
   </si>
   <si>
     <t>Barret</t>
+  </si>
+  <si>
+    <t>http://4.bp.blogspot.com/_gGLVL4FJpmM/TLyySOpRQKI/AAAAAAAAEh8/GYISAc87jDk/s1600/barret.jpg</t>
   </si>
   <si>
     <t>M60</t>
@@ -470,8 +476,8 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -510,137 +516,137 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0.357</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0.357</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0.357</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0.45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>0.357</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -652,6 +658,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -671,7 +678,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -705,57 +712,59 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -778,7 +787,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -834,81 +843,81 @@
         <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>47</v>
@@ -917,7 +926,7 @@
         <v>0.45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -958,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -975,142 +984,142 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1141,7 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1149,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1166,57 +1175,59 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1236,7 +1247,7 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1271,44 +1282,44 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>